<commit_message>
update time out Search input
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata/DataHRM.xlsx
+++ b/src/test/resources/exceldata/DataHRM.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="416">
   <si>
     <t>FIRST NAME</t>
   </si>
@@ -405,6 +405,879 @@
   </si>
   <si>
     <t>Sonny</t>
+  </si>
+  <si>
+    <t>Pete</t>
+  </si>
+  <si>
+    <t>Strosin</t>
+  </si>
+  <si>
+    <t>4b2611mw488h9anhnt</t>
+  </si>
+  <si>
+    <t>(505) 6671211</t>
+  </si>
+  <si>
+    <t>ailene.fisher@hotmail.com</t>
+  </si>
+  <si>
+    <t>aimee.walshanhnt</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Apt. 352 6567 Torp Trail, East Gerardstad, NH 21720</t>
+  </si>
+  <si>
+    <t>161 Lueilwitz Valley</t>
+  </si>
+  <si>
+    <t>East Tyronberg</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>93965</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Roob</t>
+  </si>
+  <si>
+    <t>7b8940l66j7sy1ebanhnt</t>
+  </si>
+  <si>
+    <t>(730) 6870174</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>shenita.kris@yahoo.com</t>
+  </si>
+  <si>
+    <t>onie.powlowskianhnt</t>
+  </si>
+  <si>
+    <t>67968 Will Cove, South Gina, UT 71940</t>
+  </si>
+  <si>
+    <t>5034 Sondra Cliffs</t>
+  </si>
+  <si>
+    <t>Port Sheltonland</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>26269</t>
+  </si>
+  <si>
+    <t>Cyril</t>
+  </si>
+  <si>
+    <t>Harber</t>
+  </si>
+  <si>
+    <t>21kqc561mzq3manhnt</t>
+  </si>
+  <si>
+    <t>(235) 7003189</t>
+  </si>
+  <si>
+    <t>bennie.becker@yahoo.com</t>
+  </si>
+  <si>
+    <t>donnie.zemlakanhnt</t>
+  </si>
+  <si>
+    <t>Apt. 519 9843 Ignacio Expressway, West Elke, KY 50215</t>
+  </si>
+  <si>
+    <t>88800 Alfreda Corner</t>
+  </si>
+  <si>
+    <t>Kochstad</t>
+  </si>
+  <si>
+    <t>West Virginia</t>
+  </si>
+  <si>
+    <t>65518</t>
+  </si>
+  <si>
+    <t>Cecil Kuvalis 7205</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2020-01-22</t>
+  </si>
+  <si>
+    <t>2016-06-01</t>
+  </si>
+  <si>
+    <t>Summary Project: Repellat excepturi laboriosam assumenda hic perspiciatis eaque omnis voluptate deleniti dolor unde iure expedita nulla itaque maiores eveniet eveniet sint.</t>
+  </si>
+  <si>
+    <t>Quis tempora repellat iure sit atque quos atque id vitae.</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Rayford Kris 1125</t>
+  </si>
+  <si>
+    <t>2020-03-06</t>
+  </si>
+  <si>
+    <t>2018-03-14</t>
+  </si>
+  <si>
+    <t>Summary Project: Expedita soluta accusantium quis quas laudantium omnis eveniet accusamus nihil asperiores veniam fugiat ipsum dolorum repellat temporibus praesentium itaque.</t>
+  </si>
+  <si>
+    <t>Quasi libero blanditiis officiis fugiat eum corrupti.</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>Huong Olson 4369</t>
+  </si>
+  <si>
+    <t>2020-05-04</t>
+  </si>
+  <si>
+    <t>2017-12-07</t>
+  </si>
+  <si>
+    <t>Summary Project: Perspiciatis labore culpa eos recusandae consectetur eligendi officiis eius nesciunt ipsam accusamus non cum consequuntur aliquam placeat esse unde.</t>
+  </si>
+  <si>
+    <t>Voluptatum nihil esse inventore provident laborum nulla numquam tempore dicta dolores eaque molestiae maiores.</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>Brendan Gusikowski 12190</t>
+  </si>
+  <si>
+    <t>2015-12-04</t>
+  </si>
+  <si>
+    <t>2015-06-09</t>
+  </si>
+  <si>
+    <t>Summary Task: Corporis ut fuga autem rerum doloremque laborum illum reprehenderit illo harum aspernatur ad officia a asperiores qui molestiae ducimus earum.</t>
+  </si>
+  <si>
+    <t>Description Task: Ab molestias dolor ea fugit facere odio.</t>
+  </si>
+  <si>
+    <t>Rene Ledner 93193</t>
+  </si>
+  <si>
+    <t>2022-11-21</t>
+  </si>
+  <si>
+    <t>2020-02-27</t>
+  </si>
+  <si>
+    <t>Summary Task: Aliquam sapiente vitae ad fuga quidem neque dolores aspernatur occaecati eius quisquam numquam suscipit distinctio ipsa blanditiis eligendi sit.</t>
+  </si>
+  <si>
+    <t>Description Task: Tempora recusandae cum explicabo odio vero voluptates fugiat eos deserunt vel vel.</t>
+  </si>
+  <si>
+    <t>Howard Langworth 65226</t>
+  </si>
+  <si>
+    <t>2021-12-26</t>
+  </si>
+  <si>
+    <t>2019-01-03</t>
+  </si>
+  <si>
+    <t>Summary Task: Pariatur nemo possimus non enim animi sit neque incidunt odio exercitationem cupiditate voluptas ex tempore amet nesciunt quaerat.</t>
+  </si>
+  <si>
+    <t>Description Task: Alias aliquam blanditiis atque occaecati sint aut fuga at.</t>
+  </si>
+  <si>
+    <t>Thanh</t>
+  </si>
+  <si>
+    <t>Tiffany</t>
+  </si>
+  <si>
+    <t>Abraham</t>
+  </si>
+  <si>
+    <t>Leila</t>
+  </si>
+  <si>
+    <t>Bosco</t>
+  </si>
+  <si>
+    <t>l89mu593x6panhnt</t>
+  </si>
+  <si>
+    <t>(730) 6052548</t>
+  </si>
+  <si>
+    <t>mickey.schoen@hotmail.com</t>
+  </si>
+  <si>
+    <t>leigh.satterfieldanhnt</t>
+  </si>
+  <si>
+    <t>Apt. 106 10611 Hand Forge, Goldnermouth, ND 06239</t>
+  </si>
+  <si>
+    <t>706 Naomi Ridges</t>
+  </si>
+  <si>
+    <t>New Paulitamouth</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>29766</t>
+  </si>
+  <si>
+    <t>Siobhan</t>
+  </si>
+  <si>
+    <t>Oberbrunner</t>
+  </si>
+  <si>
+    <t>229x16xoanhnt</t>
+  </si>
+  <si>
+    <t>(305) 2554452</t>
+  </si>
+  <si>
+    <t>winston.kerluke@hotmail.com</t>
+  </si>
+  <si>
+    <t>lyndon.conroyanhnt</t>
+  </si>
+  <si>
+    <t>Apt. 292 743 Bosco Drives, Lake Norine, VA 26059</t>
+  </si>
+  <si>
+    <t>892 Bartoletti Alley</t>
+  </si>
+  <si>
+    <t>Port Porfirio</t>
+  </si>
+  <si>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>51079</t>
+  </si>
+  <si>
+    <t>Margert</t>
+  </si>
+  <si>
+    <t>Wolff</t>
+  </si>
+  <si>
+    <t>8a5l7e89y41quanhnt</t>
+  </si>
+  <si>
+    <t>(305) 2019274</t>
+  </si>
+  <si>
+    <t>alina.marquardt@yahoo.com</t>
+  </si>
+  <si>
+    <t>lily.reichertanhnt</t>
+  </si>
+  <si>
+    <t>Suite 540 716 Boyd Lakes, New Tonyaport, CT 58807</t>
+  </si>
+  <si>
+    <t>21947 Anderson Pine</t>
+  </si>
+  <si>
+    <t>Hoppeton</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>77094</t>
+  </si>
+  <si>
+    <t>Dr. Clare Terry 5866</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>2019-06-01</t>
+  </si>
+  <si>
+    <t>2018-03-24</t>
+  </si>
+  <si>
+    <t>Summary Project: Laudantium id ut perspiciatis quae repellat quasi architecto cumque iusto asperiores sapiente molestias temporibus autem corporis hic expedita porro possimus fuga.</t>
+  </si>
+  <si>
+    <t>Vero ipsam voluptatum impedit quae perspiciatis porro.</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>Leticia Marquardt 9886</t>
+  </si>
+  <si>
+    <t>2017-01-17</t>
+  </si>
+  <si>
+    <t>2022-07-04</t>
+  </si>
+  <si>
+    <t>Summary Project: Autem dolores asperiores ipsam ipsum sunt aliquam explicabo eveniet aliquid incidunt quasi eos rem delectus quas atque ipsam illum cupiditate ipsam nulla at.</t>
+  </si>
+  <si>
+    <t>Maiores veniam ea unde exercitationem laborum rerum architecto nam voluptates distinctio blanditiis a.</t>
+  </si>
+  <si>
+    <t>Fredrick Stoltenberg 3528</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2021-11-12</t>
+  </si>
+  <si>
+    <t>2023-12-01</t>
+  </si>
+  <si>
+    <t>Summary Project: Laboriosam praesentium molestiae dolore odit similique provident nam mollitia consequatur dicta explicabo qui vitae quo praesentium optio.</t>
+  </si>
+  <si>
+    <t>Cumque laboriosam adipisci aliquid nobis totam provident unde inventore.</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>Rayford Stark 35960</t>
+  </si>
+  <si>
+    <t>2023-07-17</t>
+  </si>
+  <si>
+    <t>2017-07-19</t>
+  </si>
+  <si>
+    <t>Summary Task: Accusantium saepe explicabo consequatur minus eius minima veniam deleniti nam fuga rem architecto occaecati facere praesentium unde deserunt id quidem odit.</t>
+  </si>
+  <si>
+    <t>Description Task: Dolore tenetur debitis ad expedita esse dolorum repudiandae excepturi nulla eius.</t>
+  </si>
+  <si>
+    <t>Yang Dach 69417</t>
+  </si>
+  <si>
+    <t>2018-05-06</t>
+  </si>
+  <si>
+    <t>2020-09-25</t>
+  </si>
+  <si>
+    <t>Summary Task: Reiciendis nam tempore corporis porro quis eos assumenda non in nisi repellat dolor necessitatibus quidem id odio ut aperiam earum.</t>
+  </si>
+  <si>
+    <t>Description Task: Distinctio exercitationem fugit quibusdam omnis et a.</t>
+  </si>
+  <si>
+    <t>Takako Schaden 44902</t>
+  </si>
+  <si>
+    <t>2015-07-10</t>
+  </si>
+  <si>
+    <t>2024-06-20</t>
+  </si>
+  <si>
+    <t>Summary Task: At cum perferendis delectus natus accusamus quo maiores nesciunt delectus veniam ad iste in dignissimos animi tenetur aliquam eius aut quisquam.</t>
+  </si>
+  <si>
+    <t>Description Task: Laudantium corporis corrupti ea voluptate beatae minima occaecati molestiae adipisci.</t>
+  </si>
+  <si>
+    <t>Jena</t>
+  </si>
+  <si>
+    <t>Erich</t>
+  </si>
+  <si>
+    <t>Carly</t>
+  </si>
+  <si>
+    <t>Edith</t>
+  </si>
+  <si>
+    <t>Wilkinson</t>
+  </si>
+  <si>
+    <t>o43j3gs46yanhnt</t>
+  </si>
+  <si>
+    <t>(810) 5476236</t>
+  </si>
+  <si>
+    <t>alexandra.lockman@yahoo.com</t>
+  </si>
+  <si>
+    <t>arla.braunanhnt</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>614 Bruen Branch, Shelliside, KY 48652</t>
+  </si>
+  <si>
+    <t>40034 Crooks Mill</t>
+  </si>
+  <si>
+    <t>New Danettefurt</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>32079</t>
+  </si>
+  <si>
+    <t>Rex</t>
+  </si>
+  <si>
+    <t>Lehner</t>
+  </si>
+  <si>
+    <t>wghh6mp80xeooi74anhnt</t>
+  </si>
+  <si>
+    <t>(305) 4501977</t>
+  </si>
+  <si>
+    <t>providencia.rohan@hotmail.com</t>
+  </si>
+  <si>
+    <t>trevor.terryanhnt</t>
+  </si>
+  <si>
+    <t>3133 Chad Street, South Laronda, ND 89815</t>
+  </si>
+  <si>
+    <t>8368 Gerhold Mission</t>
+  </si>
+  <si>
+    <t>South Eleonorborough</t>
+  </si>
+  <si>
+    <t>North Dakota</t>
+  </si>
+  <si>
+    <t>30478</t>
+  </si>
+  <si>
+    <t>Iva</t>
+  </si>
+  <si>
+    <t>Walter</t>
+  </si>
+  <si>
+    <t>166j068x84anhnt</t>
+  </si>
+  <si>
+    <t>(279) 3154197</t>
+  </si>
+  <si>
+    <t>corey.marvin@gmail.com</t>
+  </si>
+  <si>
+    <t>joey.wehneranhnt</t>
+  </si>
+  <si>
+    <t>76778 O'Keefe Lane, North Blake, RI 44307</t>
+  </si>
+  <si>
+    <t>769 Aurea Fork</t>
+  </si>
+  <si>
+    <t>Lake Lizaville</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>20983</t>
+  </si>
+  <si>
+    <t>Trevor Rath 1801</t>
+  </si>
+  <si>
+    <t>2024-06-09</t>
+  </si>
+  <si>
+    <t>2020-05-28</t>
+  </si>
+  <si>
+    <t>Summary Project: Nobis earum ipsa esse et assumenda praesentium aut neque nemo rem rerum eius adipisci animi consectetur.</t>
+  </si>
+  <si>
+    <t>Ducimus recusandae nostrum hic sint numquam ratione autem quis dignissimos error.</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>Rene Quitzon II 279</t>
+  </si>
+  <si>
+    <t>2022-02-25</t>
+  </si>
+  <si>
+    <t>2018-07-06</t>
+  </si>
+  <si>
+    <t>Summary Project: Quisquam ratione ea sint aliquam ducimus nisi dicta occaecati nihil dolore eaque exercitationem illum qui voluptate voluptates ea debitis totam odio qui.</t>
+  </si>
+  <si>
+    <t>Sed doloribus fuga facere similique sed voluptates saepe iste non ipsam consectetur.</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Shan Williamson MD 2490</t>
+  </si>
+  <si>
+    <t>2021-12-14</t>
+  </si>
+  <si>
+    <t>2024-02-18</t>
+  </si>
+  <si>
+    <t>Summary Project: Voluptate id odit voluptatum dolorem voluptas exercitationem nihil aperiam reprehenderit ea culpa quod magni omnis quia eius at atque non consequatur.</t>
+  </si>
+  <si>
+    <t>Facilis ab quibusdam quasi laborum fugit deleniti.</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Noel Schamberger III 90174</t>
+  </si>
+  <si>
+    <t>2023-04-16</t>
+  </si>
+  <si>
+    <t>2015-02-07</t>
+  </si>
+  <si>
+    <t>Summary Task: Adipisci ipsum asperiores nesciunt saepe suscipit repellendus dolore quaerat ducimus expedita corrupti iusto repellat qui hic velit ipsum facilis magnam totam.</t>
+  </si>
+  <si>
+    <t>Description Task: Animi accusantium magni ratione nobis nulla quos accusantium dolore repellat.</t>
+  </si>
+  <si>
+    <t>Ms. Clementine Nader 41524</t>
+  </si>
+  <si>
+    <t>2017-12-09</t>
+  </si>
+  <si>
+    <t>2018-05-14</t>
+  </si>
+  <si>
+    <t>Summary Task: Enim magnam sequi at quam praesentium blanditiis beatae est explicabo repellendus sequi nisi placeat tempore deserunt quod reprehenderit magni.</t>
+  </si>
+  <si>
+    <t>Description Task: Expedita quos excepturi iusto dolorum laboriosam occaecati vel architecto.</t>
+  </si>
+  <si>
+    <t>Kerry Marks 22214</t>
+  </si>
+  <si>
+    <t>2016-07-12</t>
+  </si>
+  <si>
+    <t>2016-10-14</t>
+  </si>
+  <si>
+    <t>Summary Task: Libero earum ratione sunt fugiat autem harum neque magnam eaque doloremque adipisci molestias exercitationem expedita culpa mollitia dicta ex amet vero quod.</t>
+  </si>
+  <si>
+    <t>Description Task: Necessitatibus exercitationem atque adipisci recusandae aut numquam id quos distinctio.</t>
+  </si>
+  <si>
+    <t>Justin</t>
+  </si>
+  <si>
+    <t>Hyun</t>
+  </si>
+  <si>
+    <t>Val</t>
+  </si>
+  <si>
+    <t>Basilia</t>
+  </si>
+  <si>
+    <t>Koch</t>
+  </si>
+  <si>
+    <t>csifat3u723lheweanhnt</t>
+  </si>
+  <si>
+    <t>(472) 2004791</t>
+  </si>
+  <si>
+    <t>micheal.keebler@hotmail.com</t>
+  </si>
+  <si>
+    <t>marty.stromananhnt</t>
+  </si>
+  <si>
+    <t>61242 Robt Valley, New Youngfurt, ME 57191</t>
+  </si>
+  <si>
+    <t>4275 Mabel Creek</t>
+  </si>
+  <si>
+    <t>North Josephina</t>
+  </si>
+  <si>
+    <t>89034</t>
+  </si>
+  <si>
+    <t>Jackelyn</t>
+  </si>
+  <si>
+    <t>Stark</t>
+  </si>
+  <si>
+    <t>dorcbau1jr7xu6anhnt</t>
+  </si>
+  <si>
+    <t>(931) 2589805</t>
+  </si>
+  <si>
+    <t>dena.streich@gmail.com</t>
+  </si>
+  <si>
+    <t>kendall.binsanhnt</t>
+  </si>
+  <si>
+    <t>571 Stark Fords, Rohanborough, RI 94076</t>
+  </si>
+  <si>
+    <t>41511 Clarice Motorway</t>
+  </si>
+  <si>
+    <t>Lake Letitiaburgh</t>
+  </si>
+  <si>
+    <t>76708</t>
+  </si>
+  <si>
+    <t>Sherise</t>
+  </si>
+  <si>
+    <t>Feeney</t>
+  </si>
+  <si>
+    <t>0aj40bg15m9ianhnt</t>
+  </si>
+  <si>
+    <t>(305) 2031719</t>
+  </si>
+  <si>
+    <t>risa.sanford@hotmail.com</t>
+  </si>
+  <si>
+    <t>byron.volkmananhnt</t>
+  </si>
+  <si>
+    <t>5728 Grady Center, Chastown, KS 61708</t>
+  </si>
+  <si>
+    <t>91058 Logan Stream</t>
+  </si>
+  <si>
+    <t>South Noahton</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>80216</t>
+  </si>
+  <si>
+    <t>Silvia Predovic 529</t>
+  </si>
+  <si>
+    <t>2016-01-02</t>
+  </si>
+  <si>
+    <t>2017-01-29</t>
+  </si>
+  <si>
+    <t>Summary Project: Beatae modi numquam accusamus pariatur dignissimos facere quos unde nemo iure perferendis est delectus odit autem necessitatibus porro facere quidem.</t>
+  </si>
+  <si>
+    <t>Nobis magni voluptas dolorum voluptate placeat fuga ullam delectus nam suscipit quos vitae.</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>Mr. Marion Kshlerin 3423</t>
+  </si>
+  <si>
+    <t>2017-01-13</t>
+  </si>
+  <si>
+    <t>2020-08-05</t>
+  </si>
+  <si>
+    <t>Summary Project: Omnis laboriosam veniam assumenda sunt adipisci ipsum necessitatibus officia mollitia numquam occaecati deserunt mollitia occaecati minima.</t>
+  </si>
+  <si>
+    <t>Esse harum eaque libero dolor omnis neque veritatis inventore.</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Moises Kilback 319</t>
+  </si>
+  <si>
+    <t>2016-09-23</t>
+  </si>
+  <si>
+    <t>Summary Project: Consectetur illum earum quod accusantium et maiores omnis vitae maiores nihil distinctio illum voluptate expedita dicta molestiae nostrum tempora.</t>
+  </si>
+  <si>
+    <t>Molestiae temporibus excepturi delectus vitae possimus cumque omnis expedita consectetur natus.</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Fleta Nader 69050</t>
+  </si>
+  <si>
+    <t>2022-01-25</t>
+  </si>
+  <si>
+    <t>2023-08-30</t>
+  </si>
+  <si>
+    <t>Summary Task: Aliquid laboriosam enim inventore vero itaque excepturi quasi incidunt mollitia tempore laborum corporis reprehenderit in nisi voluptatem molestiae molestias consectetur.</t>
+  </si>
+  <si>
+    <t>Description Task: Laborum voluptates qui aperiam mollitia quas adipisci deserunt nihil earum error.</t>
+  </si>
+  <si>
+    <t>Tori Mohr 6174</t>
+  </si>
+  <si>
+    <t>2017-12-19</t>
+  </si>
+  <si>
+    <t>2023-06-30</t>
+  </si>
+  <si>
+    <t>Summary Task: Excepturi fuga quas enim harum deleniti cupiditate facilis excepturi quasi doloribus facere sunt voluptatibus quaerat vitae quasi cum accusantium natus unde libero.</t>
+  </si>
+  <si>
+    <t>Description Task: Cupiditate incidunt velit deleniti architecto perferendis at voluptas maiores aliquid autem aspernatur magni dolorem.</t>
+  </si>
+  <si>
+    <t>Cristobal Anderson 79751</t>
+  </si>
+  <si>
+    <t>2016-12-18</t>
+  </si>
+  <si>
+    <t>2016-04-14</t>
+  </si>
+  <si>
+    <t>Summary Task: Ullam accusantium vel voluptatem aut esse commodi autem corrupti molestias impedit quaerat odit quas accusantium voluptatum necessitatibus.</t>
+  </si>
+  <si>
+    <t>Description Task: Iste accusamus aliquam veniam doloremque voluptatum natus quod nulla reiciendis est adipisci accusamus.</t>
+  </si>
+  <si>
+    <t>Arthur</t>
+  </si>
+  <si>
+    <t>Randy</t>
+  </si>
+  <si>
+    <t>Avery</t>
   </si>
 </sst>
 </file>
@@ -456,10 +1329,1486 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="618">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1228,143 +3577,143 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="3">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s" s="4">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s" s="5">
-        <v>31</v>
-      </c>
-      <c r="D2" t="s" s="6">
-        <v>32</v>
-      </c>
-      <c r="E2" t="s" s="7">
+      <c r="A2" t="s" s="495">
+        <v>347</v>
+      </c>
+      <c r="B2" t="s" s="496">
+        <v>348</v>
+      </c>
+      <c r="C2" t="s" s="497">
+        <v>349</v>
+      </c>
+      <c r="D2" t="s" s="498">
+        <v>350</v>
+      </c>
+      <c r="E2" t="s" s="499">
         <v>33</v>
       </c>
-      <c r="F2" t="s" s="8">
-        <v>34</v>
-      </c>
-      <c r="G2" t="s" s="9">
-        <v>35</v>
-      </c>
-      <c r="H2" t="s" s="10">
-        <v>36</v>
-      </c>
-      <c r="I2" t="s" s="11">
-        <v>37</v>
-      </c>
-      <c r="J2" t="s" s="12">
-        <v>38</v>
-      </c>
-      <c r="K2" t="s" s="13">
-        <v>39</v>
-      </c>
-      <c r="L2" t="s" s="14">
-        <v>40</v>
-      </c>
-      <c r="M2" t="s" s="15">
-        <v>41</v>
-      </c>
-      <c r="N2" t="s" s="16">
-        <v>42</v>
-      </c>
-      <c r="O2" t="s" s="17">
+      <c r="F2" t="s" s="500">
+        <v>351</v>
+      </c>
+      <c r="G2" t="s" s="501">
+        <v>352</v>
+      </c>
+      <c r="H2" t="s" s="502">
+        <v>131</v>
+      </c>
+      <c r="I2" t="s" s="503">
+        <v>353</v>
+      </c>
+      <c r="J2" t="s" s="504">
+        <v>354</v>
+      </c>
+      <c r="K2" t="s" s="505">
+        <v>355</v>
+      </c>
+      <c r="L2" t="s" s="506">
+        <v>305</v>
+      </c>
+      <c r="M2" t="s" s="507">
+        <v>356</v>
+      </c>
+      <c r="N2" t="s" s="508">
+        <v>56</v>
+      </c>
+      <c r="O2" t="s" s="509">
         <v>43</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="18">
-        <v>44</v>
-      </c>
-      <c r="B3" t="s" s="19">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s" s="20">
-        <v>46</v>
-      </c>
-      <c r="D3" t="s" s="21">
-        <v>47</v>
-      </c>
-      <c r="E3" t="s" s="22">
-        <v>33</v>
-      </c>
-      <c r="F3" t="s" s="23">
-        <v>48</v>
-      </c>
-      <c r="G3" t="s" s="24">
-        <v>49</v>
-      </c>
-      <c r="H3" t="s" s="25">
-        <v>50</v>
-      </c>
-      <c r="I3" t="s" s="26">
-        <v>51</v>
-      </c>
-      <c r="J3" t="s" s="27">
-        <v>52</v>
-      </c>
-      <c r="K3" t="s" s="28">
-        <v>53</v>
-      </c>
-      <c r="L3" t="s" s="29">
-        <v>54</v>
-      </c>
-      <c r="M3" t="s" s="30">
-        <v>55</v>
-      </c>
-      <c r="N3" t="s" s="31">
-        <v>56</v>
-      </c>
-      <c r="O3" t="s" s="32">
+      <c r="A3" t="s" s="510">
+        <v>357</v>
+      </c>
+      <c r="B3" t="s" s="511">
+        <v>358</v>
+      </c>
+      <c r="C3" t="s" s="512">
+        <v>359</v>
+      </c>
+      <c r="D3" t="s" s="513">
+        <v>360</v>
+      </c>
+      <c r="E3" t="s" s="514">
+        <v>141</v>
+      </c>
+      <c r="F3" t="s" s="515">
+        <v>361</v>
+      </c>
+      <c r="G3" t="s" s="516">
+        <v>362</v>
+      </c>
+      <c r="H3" t="s" s="517">
+        <v>63</v>
+      </c>
+      <c r="I3" t="s" s="518">
+        <v>363</v>
+      </c>
+      <c r="J3" t="s" s="519">
+        <v>364</v>
+      </c>
+      <c r="K3" t="s" s="520">
+        <v>365</v>
+      </c>
+      <c r="L3" t="s" s="521">
+        <v>40</v>
+      </c>
+      <c r="M3" t="s" s="522">
+        <v>366</v>
+      </c>
+      <c r="N3" t="s" s="523">
+        <v>42</v>
+      </c>
+      <c r="O3" t="s" s="524">
         <v>43</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="33">
-        <v>57</v>
-      </c>
-      <c r="B4" t="s" s="34">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s" s="35">
-        <v>59</v>
-      </c>
-      <c r="D4" t="s" s="36">
-        <v>60</v>
-      </c>
-      <c r="E4" t="s" s="37">
-        <v>33</v>
-      </c>
-      <c r="F4" t="s" s="38">
-        <v>61</v>
-      </c>
-      <c r="G4" t="s" s="39">
-        <v>62</v>
-      </c>
-      <c r="H4" t="s" s="40">
-        <v>63</v>
-      </c>
-      <c r="I4" t="s" s="41">
-        <v>64</v>
-      </c>
-      <c r="J4" t="s" s="42">
-        <v>65</v>
-      </c>
-      <c r="K4" t="s" s="43">
-        <v>66</v>
-      </c>
-      <c r="L4" t="s" s="44">
-        <v>67</v>
-      </c>
-      <c r="M4" t="s" s="45">
-        <v>68</v>
-      </c>
-      <c r="N4" t="s" s="46">
-        <v>56</v>
-      </c>
-      <c r="O4" t="s" s="47">
+      <c r="A4" t="s" s="525">
+        <v>367</v>
+      </c>
+      <c r="B4" t="s" s="526">
+        <v>368</v>
+      </c>
+      <c r="C4" t="s" s="527">
+        <v>369</v>
+      </c>
+      <c r="D4" t="s" s="528">
+        <v>370</v>
+      </c>
+      <c r="E4" t="s" s="529">
+        <v>141</v>
+      </c>
+      <c r="F4" t="s" s="530">
+        <v>371</v>
+      </c>
+      <c r="G4" t="s" s="531">
+        <v>372</v>
+      </c>
+      <c r="H4" t="s" s="532">
+        <v>279</v>
+      </c>
+      <c r="I4" t="s" s="533">
+        <v>373</v>
+      </c>
+      <c r="J4" t="s" s="534">
+        <v>374</v>
+      </c>
+      <c r="K4" t="s" s="535">
+        <v>375</v>
+      </c>
+      <c r="L4" t="s" s="536">
+        <v>376</v>
+      </c>
+      <c r="M4" t="s" s="537">
+        <v>377</v>
+      </c>
+      <c r="N4" t="s" s="538">
+        <v>42</v>
+      </c>
+      <c r="O4" t="s" s="539">
         <v>43</v>
       </c>
     </row>
@@ -1427,108 +3776,108 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="48">
-        <v>69</v>
-      </c>
-      <c r="B2" t="s" s="49">
+      <c r="A2" t="s" s="540">
+        <v>378</v>
+      </c>
+      <c r="B2" t="s" s="541">
         <v>70</v>
       </c>
-      <c r="C2" t="s" s="50">
-        <v>71</v>
-      </c>
-      <c r="D2" t="s" s="51">
-        <v>72</v>
-      </c>
-      <c r="E2" t="s" s="52">
-        <v>73</v>
-      </c>
-      <c r="F2" t="s" s="53">
-        <v>74</v>
-      </c>
-      <c r="G2" t="s" s="54">
-        <v>75</v>
-      </c>
-      <c r="H2" t="s" s="55">
+      <c r="C2" t="s" s="542">
+        <v>114</v>
+      </c>
+      <c r="D2" t="s" s="543">
+        <v>90</v>
+      </c>
+      <c r="E2" t="s" s="544">
+        <v>379</v>
+      </c>
+      <c r="F2" t="s" s="545">
+        <v>380</v>
+      </c>
+      <c r="G2" t="s" s="546">
+        <v>381</v>
+      </c>
+      <c r="H2" t="s" s="547">
         <v>76</v>
       </c>
-      <c r="I2" t="s" s="56">
-        <v>77</v>
-      </c>
-      <c r="J2" t="s" s="57">
-        <v>78</v>
-      </c>
-      <c r="K2" t="s" s="58">
-        <v>79</v>
+      <c r="I2" t="s" s="548">
+        <v>382</v>
+      </c>
+      <c r="J2" t="s" s="549">
+        <v>383</v>
+      </c>
+      <c r="K2" t="s" s="550">
+        <v>88</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="59">
-        <v>80</v>
-      </c>
-      <c r="B3" t="s" s="60">
+      <c r="A3" t="s" s="551">
+        <v>384</v>
+      </c>
+      <c r="B3" t="s" s="552">
         <v>70</v>
       </c>
-      <c r="C3" t="s" s="61">
-        <v>81</v>
-      </c>
-      <c r="D3" t="s" s="62">
-        <v>72</v>
-      </c>
-      <c r="E3" t="s" s="63">
-        <v>82</v>
-      </c>
-      <c r="F3" t="s" s="64">
-        <v>83</v>
-      </c>
-      <c r="G3" t="s" s="65">
-        <v>84</v>
-      </c>
-      <c r="H3" t="s" s="66">
+      <c r="C3" t="s" s="553">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s" s="554">
+        <v>100</v>
+      </c>
+      <c r="E3" t="s" s="555">
+        <v>385</v>
+      </c>
+      <c r="F3" t="s" s="556">
+        <v>386</v>
+      </c>
+      <c r="G3" t="s" s="557">
+        <v>387</v>
+      </c>
+      <c r="H3" t="s" s="558">
         <v>85</v>
       </c>
-      <c r="I3" t="s" s="67">
-        <v>86</v>
-      </c>
-      <c r="J3" t="s" s="68">
-        <v>87</v>
-      </c>
-      <c r="K3" t="s" s="69">
-        <v>88</v>
+      <c r="I3" t="s" s="559">
+        <v>388</v>
+      </c>
+      <c r="J3" t="s" s="560">
+        <v>389</v>
+      </c>
+      <c r="K3" t="s" s="561">
+        <v>167</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="70">
-        <v>89</v>
-      </c>
-      <c r="B4" t="s" s="71">
+      <c r="A4" t="s" s="562">
+        <v>390</v>
+      </c>
+      <c r="B4" t="s" s="563">
         <v>70</v>
       </c>
-      <c r="C4" t="s" s="72">
-        <v>71</v>
-      </c>
-      <c r="D4" t="s" s="73">
-        <v>90</v>
-      </c>
-      <c r="E4" t="s" s="74">
-        <v>91</v>
-      </c>
-      <c r="F4" t="s" s="75">
-        <v>92</v>
-      </c>
-      <c r="G4" t="s" s="76">
-        <v>93</v>
-      </c>
-      <c r="H4" t="s" s="77">
-        <v>85</v>
-      </c>
-      <c r="I4" t="s" s="78">
-        <v>94</v>
-      </c>
-      <c r="J4" t="s" s="79">
-        <v>95</v>
-      </c>
-      <c r="K4" t="s" s="80">
-        <v>79</v>
+      <c r="C4" t="s" s="564">
+        <v>108</v>
+      </c>
+      <c r="D4" t="s" s="565">
+        <v>103</v>
+      </c>
+      <c r="E4" t="s" s="566">
+        <v>261</v>
+      </c>
+      <c r="F4" t="s" s="567">
+        <v>391</v>
+      </c>
+      <c r="G4" t="s" s="568">
+        <v>392</v>
+      </c>
+      <c r="H4" t="s" s="569">
+        <v>76</v>
+      </c>
+      <c r="I4" t="s" s="570">
+        <v>393</v>
+      </c>
+      <c r="J4" t="s" s="571">
+        <v>394</v>
+      </c>
+      <c r="K4" t="s" s="572">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1561,45 +3910,45 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="81">
+      <c r="A2" t="s" s="573">
         <v>96</v>
       </c>
-      <c r="B2" t="s" s="82">
+      <c r="B2" t="s" s="574">
         <v>90</v>
       </c>
-      <c r="C2" t="s" s="83">
-        <v>97</v>
-      </c>
-      <c r="D2" t="s" s="84">
-        <v>98</v>
+      <c r="C2" t="s" s="575">
+        <v>319</v>
+      </c>
+      <c r="D2" t="s" s="576">
+        <v>395</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="85">
+      <c r="A3" t="s" s="577">
         <v>99</v>
       </c>
-      <c r="B3" t="s" s="86">
-        <v>100</v>
-      </c>
-      <c r="C3" t="s" s="87">
-        <v>97</v>
-      </c>
-      <c r="D3" t="s" s="88">
-        <v>101</v>
+      <c r="B3" t="s" s="578">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s" s="579">
+        <v>88</v>
+      </c>
+      <c r="D3" t="s" s="580">
+        <v>396</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="89">
+      <c r="A4" t="s" s="581">
         <v>102</v>
       </c>
-      <c r="B4" t="s" s="90">
-        <v>103</v>
-      </c>
-      <c r="C4" t="s" s="91">
-        <v>97</v>
-      </c>
-      <c r="D4" t="s" s="92">
-        <v>104</v>
+      <c r="B4" t="s" s="582">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s" s="583">
+        <v>88</v>
+      </c>
+      <c r="D4" t="s" s="584">
+        <v>397</v>
       </c>
     </row>
   </sheetData>
@@ -1652,81 +4001,81 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="93">
+      <c r="A2" t="s" s="585">
         <v>96</v>
       </c>
-      <c r="B2" t="s" s="94">
-        <v>105</v>
-      </c>
-      <c r="C2" t="s" s="95">
-        <v>106</v>
-      </c>
-      <c r="D2" t="s" s="96">
-        <v>107</v>
-      </c>
-      <c r="E2" t="s" s="97">
-        <v>108</v>
-      </c>
-      <c r="F2" t="s" s="98">
-        <v>109</v>
-      </c>
-      <c r="G2" t="s" s="99">
-        <v>110</v>
-      </c>
-      <c r="H2" t="s" s="100">
+      <c r="B2" t="s" s="586">
+        <v>398</v>
+      </c>
+      <c r="C2" t="s" s="587">
+        <v>399</v>
+      </c>
+      <c r="D2" t="s" s="588">
+        <v>400</v>
+      </c>
+      <c r="E2" t="s" s="589">
+        <v>161</v>
+      </c>
+      <c r="F2" t="s" s="590">
+        <v>401</v>
+      </c>
+      <c r="G2" t="s" s="591">
+        <v>402</v>
+      </c>
+      <c r="H2" t="s" s="592">
         <v>76</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="101">
+      <c r="A3" t="s" s="593">
         <v>99</v>
       </c>
-      <c r="B3" t="s" s="102">
-        <v>111</v>
-      </c>
-      <c r="C3" t="s" s="103">
-        <v>112</v>
-      </c>
-      <c r="D3" t="s" s="104">
-        <v>113</v>
-      </c>
-      <c r="E3" t="s" s="105">
-        <v>114</v>
-      </c>
-      <c r="F3" t="s" s="106">
-        <v>115</v>
-      </c>
-      <c r="G3" t="s" s="107">
-        <v>116</v>
-      </c>
-      <c r="H3" t="s" s="108">
+      <c r="B3" t="s" s="594">
+        <v>403</v>
+      </c>
+      <c r="C3" t="s" s="595">
+        <v>404</v>
+      </c>
+      <c r="D3" t="s" s="596">
+        <v>405</v>
+      </c>
+      <c r="E3" t="s" s="597">
+        <v>235</v>
+      </c>
+      <c r="F3" t="s" s="598">
+        <v>406</v>
+      </c>
+      <c r="G3" t="s" s="599">
+        <v>407</v>
+      </c>
+      <c r="H3" t="s" s="600">
         <v>76</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="109">
+      <c r="A4" t="s" s="601">
         <v>102</v>
       </c>
-      <c r="B4" t="s" s="110">
-        <v>117</v>
-      </c>
-      <c r="C4" t="s" s="111">
-        <v>118</v>
-      </c>
-      <c r="D4" t="s" s="112">
-        <v>119</v>
-      </c>
-      <c r="E4" t="s" s="113">
-        <v>101</v>
-      </c>
-      <c r="F4" t="s" s="114">
-        <v>120</v>
-      </c>
-      <c r="G4" t="s" s="115">
-        <v>121</v>
-      </c>
-      <c r="H4" t="s" s="116">
-        <v>76</v>
+      <c r="B4" t="s" s="602">
+        <v>408</v>
+      </c>
+      <c r="C4" t="s" s="603">
+        <v>409</v>
+      </c>
+      <c r="D4" t="s" s="604">
+        <v>410</v>
+      </c>
+      <c r="E4" t="s" s="605">
+        <v>235</v>
+      </c>
+      <c r="F4" t="s" s="606">
+        <v>411</v>
+      </c>
+      <c r="G4" t="s" s="607">
+        <v>412</v>
+      </c>
+      <c r="H4" t="s" s="608">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1761,35 +4110,35 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="117">
+      <c r="A2" t="s" s="609">
         <v>96</v>
       </c>
-      <c r="B2" t="s" s="118">
-        <v>122</v>
-      </c>
-      <c r="C2" t="s" s="119">
+      <c r="B2" t="s" s="610">
+        <v>413</v>
+      </c>
+      <c r="C2" t="s" s="611">
         <v>43</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="120">
+      <c r="A3" t="s" s="612">
         <v>99</v>
       </c>
-      <c r="B3" t="s" s="121">
-        <v>123</v>
-      </c>
-      <c r="C3" t="s" s="122">
+      <c r="B3" t="s" s="613">
+        <v>414</v>
+      </c>
+      <c r="C3" t="s" s="614">
         <v>43</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="123">
+      <c r="A4" t="s" s="615">
         <v>102</v>
       </c>
-      <c r="B4" t="s" s="124">
-        <v>124</v>
-      </c>
-      <c r="C4" t="s" s="125">
+      <c r="B4" t="s" s="616">
+        <v>415</v>
+      </c>
+      <c r="C4" t="s" s="617">
         <v>43</v>
       </c>
     </row>

</xml_diff>